<commit_message>
Added TripProductValidations On ConfirmationPage For Hotel
</commit_message>
<xml_diff>
--- a/Rovia.UI.Automation.Tests/DataSheet/Hotel/HotelScenarios.xlsx
+++ b/Rovia.UI.Automation.Tests/DataSheet/Hotel/HotelScenarios.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="743" uniqueCount="103">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="799" uniqueCount="106">
   <si>
     <t>Description</t>
   </si>
@@ -332,6 +332,15 @@
   </si>
   <si>
     <t>AMENITIES</t>
+  </si>
+  <si>
+    <t>Search|AddToCart|CHECKOUTTRIP|LOGIN|ENTERPAXINFO|CONFIRMPAXINFO|PayNOW</t>
+  </si>
+  <si>
+    <t>PaymentMode</t>
+  </si>
+  <si>
+    <t>CreditCard</t>
   </si>
 </sst>
 </file>
@@ -529,7 +538,124 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="200">
+  <dxfs count="209">
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right/>
+        <top/>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right/>
+        <top/>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right/>
+        <top/>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right/>
+        <top/>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right/>
+        <top/>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right/>
+        <top/>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right/>
+        <top/>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right/>
+        <top/>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right/>
+        <top/>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
     <dxf>
       <numFmt numFmtId="30" formatCode="@"/>
       <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -802,30 +928,30 @@
       </border>
     </dxf>
     <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
       <border>
         <bottom style="thin">
           <color indexed="64"/>
         </bottom>
       </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <border diagonalUp="0" diagonalDown="0">
@@ -3691,270 +3817,279 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table2" displayName="Table2" ref="A1:O38" totalsRowShown="0" headerRowDxfId="199" dataDxfId="197" headerRowBorderDxfId="198" tableBorderDxfId="196" totalsRowBorderDxfId="195">
-  <autoFilter ref="A1:O38"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table2" displayName="Table2" ref="A1:P38" totalsRowShown="0" headerRowDxfId="208" dataDxfId="206" headerRowBorderDxfId="207" tableBorderDxfId="205" totalsRowBorderDxfId="204">
+  <autoFilter ref="A1:P38"/>
   <sortState ref="A2:O38">
     <sortCondition ref="L1:L38"/>
   </sortState>
-  <tableColumns count="15">
-    <tableColumn id="1" name="Description" dataDxfId="194"/>
-    <tableColumn id="16" name="ExecutionPipeLine" dataDxfId="193"/>
-    <tableColumn id="17" name="CheckInDate" dataDxfId="192"/>
-    <tableColumn id="18" name="CheckOutDate" dataDxfId="191"/>
-    <tableColumn id="3" name="ShortLocation" dataDxfId="190"/>
-    <tableColumn id="4" name="Location" dataDxfId="189"/>
-    <tableColumn id="5" name="Adults" dataDxfId="188"/>
-    <tableColumn id="6" name="ChildrenAges" dataDxfId="187"/>
-    <tableColumn id="8" name="AdditionalPreferences" dataDxfId="186"/>
-    <tableColumn id="9" name="HotelName" dataDxfId="185"/>
-    <tableColumn id="10" name="StarRating" dataDxfId="184"/>
-    <tableColumn id="11" name="Supplier" dataDxfId="183"/>
-    <tableColumn id="7" name="UserType" dataDxfId="182"/>
-    <tableColumn id="14" name="PostSearchFilters" dataDxfId="181"/>
-    <tableColumn id="15" name="PostSearchFilterValues" dataDxfId="180"/>
+  <tableColumns count="16">
+    <tableColumn id="1" name="Description" dataDxfId="203"/>
+    <tableColumn id="16" name="ExecutionPipeLine" dataDxfId="202"/>
+    <tableColumn id="17" name="CheckInDate" dataDxfId="201"/>
+    <tableColumn id="18" name="CheckOutDate" dataDxfId="200"/>
+    <tableColumn id="3" name="ShortLocation" dataDxfId="199"/>
+    <tableColumn id="4" name="Location" dataDxfId="198"/>
+    <tableColumn id="5" name="Adults" dataDxfId="197"/>
+    <tableColumn id="6" name="ChildrenAges" dataDxfId="196"/>
+    <tableColumn id="8" name="AdditionalPreferences" dataDxfId="195"/>
+    <tableColumn id="9" name="HotelName" dataDxfId="194"/>
+    <tableColumn id="10" name="StarRating" dataDxfId="193"/>
+    <tableColumn id="11" name="Supplier" dataDxfId="192"/>
+    <tableColumn id="7" name="UserType" dataDxfId="191"/>
+    <tableColumn id="2" name="PaymentMode" dataDxfId="7"/>
+    <tableColumn id="14" name="PostSearchFilters" dataDxfId="190"/>
+    <tableColumn id="15" name="PostSearchFilterValues" dataDxfId="189"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table10.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="10" name="Table21011" displayName="Table21011" ref="A1:O17" totalsRowShown="0" headerRowDxfId="39" dataDxfId="37" headerRowBorderDxfId="38" tableBorderDxfId="36" totalsRowBorderDxfId="35">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="10" name="Table21011" displayName="Table21011" ref="A1:O17" totalsRowShown="0" headerRowDxfId="28" dataDxfId="26" headerRowBorderDxfId="27" tableBorderDxfId="25" totalsRowBorderDxfId="24">
   <autoFilter ref="A1:O17"/>
   <sortState ref="A2:O38">
     <sortCondition ref="L1:L38"/>
   </sortState>
   <tableColumns count="15">
-    <tableColumn id="1" name="Description" dataDxfId="34"/>
-    <tableColumn id="16" name="ExecutionPipeLine" dataDxfId="33"/>
-    <tableColumn id="17" name="CheckInDate" dataDxfId="32"/>
-    <tableColumn id="18" name="CheckOutDate" dataDxfId="31"/>
-    <tableColumn id="3" name="ShortLocation" dataDxfId="30"/>
-    <tableColumn id="4" name="Location" dataDxfId="29"/>
-    <tableColumn id="5" name="Adults" dataDxfId="28"/>
-    <tableColumn id="6" name="ChildrenAges" dataDxfId="27"/>
-    <tableColumn id="8" name="AdditionalPreferences" dataDxfId="26"/>
-    <tableColumn id="9" name="HotelName" dataDxfId="25"/>
-    <tableColumn id="10" name="StarRating" dataDxfId="24"/>
-    <tableColumn id="11" name="Supplier" dataDxfId="23"/>
-    <tableColumn id="7" name="UserType" dataDxfId="22"/>
-    <tableColumn id="14" name="PostSearchFilters" dataDxfId="21"/>
-    <tableColumn id="15" name="PostSearchFilterValues" dataDxfId="20"/>
+    <tableColumn id="1" name="Description" dataDxfId="23"/>
+    <tableColumn id="16" name="ExecutionPipeLine" dataDxfId="22"/>
+    <tableColumn id="17" name="CheckInDate" dataDxfId="21"/>
+    <tableColumn id="18" name="CheckOutDate" dataDxfId="20"/>
+    <tableColumn id="3" name="ShortLocation" dataDxfId="19"/>
+    <tableColumn id="4" name="Location" dataDxfId="18"/>
+    <tableColumn id="5" name="Adults" dataDxfId="17"/>
+    <tableColumn id="6" name="ChildrenAges" dataDxfId="16"/>
+    <tableColumn id="8" name="AdditionalPreferences" dataDxfId="15"/>
+    <tableColumn id="9" name="HotelName" dataDxfId="14"/>
+    <tableColumn id="10" name="StarRating" dataDxfId="13"/>
+    <tableColumn id="11" name="Supplier" dataDxfId="12"/>
+    <tableColumn id="7" name="UserType" dataDxfId="11"/>
+    <tableColumn id="14" name="PostSearchFilters" dataDxfId="10"/>
+    <tableColumn id="15" name="PostSearchFilterValues" dataDxfId="9"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table23" displayName="Table23" ref="A1:O2" totalsRowShown="0" headerRowDxfId="179" dataDxfId="177" headerRowBorderDxfId="178" tableBorderDxfId="176" totalsRowBorderDxfId="175">
-  <autoFilter ref="A1:O2"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table23" displayName="Table23" ref="A1:P2" totalsRowShown="0" headerRowDxfId="188" dataDxfId="186" headerRowBorderDxfId="187" tableBorderDxfId="185" totalsRowBorderDxfId="184">
+  <autoFilter ref="A1:P2"/>
   <sortState ref="A2:O38">
     <sortCondition ref="L1:L38"/>
   </sortState>
-  <tableColumns count="15">
-    <tableColumn id="1" name="Description" dataDxfId="174"/>
-    <tableColumn id="16" name="ExecutionPipeLine" dataDxfId="173"/>
-    <tableColumn id="17" name="CheckInDate" dataDxfId="172"/>
-    <tableColumn id="18" name="CheckOutDate" dataDxfId="171"/>
-    <tableColumn id="3" name="ShortLocation" dataDxfId="170"/>
-    <tableColumn id="4" name="Location" dataDxfId="169"/>
-    <tableColumn id="5" name="Adults" dataDxfId="168"/>
-    <tableColumn id="6" name="ChildrenAges" dataDxfId="167"/>
-    <tableColumn id="8" name="AdditionalPreferences" dataDxfId="166"/>
-    <tableColumn id="9" name="HotelName" dataDxfId="165"/>
-    <tableColumn id="10" name="StarRating" dataDxfId="164"/>
-    <tableColumn id="11" name="Supplier" dataDxfId="163"/>
-    <tableColumn id="7" name="UserType" dataDxfId="162"/>
-    <tableColumn id="14" name="PostSearchFilters" dataDxfId="161"/>
-    <tableColumn id="15" name="PostSearchFilterValues" dataDxfId="160"/>
+  <tableColumns count="16">
+    <tableColumn id="1" name="Description" dataDxfId="183"/>
+    <tableColumn id="16" name="ExecutionPipeLine" dataDxfId="182"/>
+    <tableColumn id="17" name="CheckInDate" dataDxfId="181"/>
+    <tableColumn id="18" name="CheckOutDate" dataDxfId="180"/>
+    <tableColumn id="3" name="ShortLocation" dataDxfId="179"/>
+    <tableColumn id="4" name="Location" dataDxfId="178"/>
+    <tableColumn id="5" name="Adults" dataDxfId="177"/>
+    <tableColumn id="6" name="ChildrenAges" dataDxfId="176"/>
+    <tableColumn id="8" name="AdditionalPreferences" dataDxfId="175"/>
+    <tableColumn id="9" name="HotelName" dataDxfId="174"/>
+    <tableColumn id="10" name="StarRating" dataDxfId="173"/>
+    <tableColumn id="11" name="Supplier" dataDxfId="172"/>
+    <tableColumn id="7" name="UserType" dataDxfId="171"/>
+    <tableColumn id="2" name="PaymentMode" dataDxfId="6"/>
+    <tableColumn id="14" name="PostSearchFilters" dataDxfId="170"/>
+    <tableColumn id="15" name="PostSearchFilterValues" dataDxfId="169"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table24" displayName="Table24" ref="A1:O5" totalsRowShown="0" headerRowDxfId="159" dataDxfId="157" headerRowBorderDxfId="158" tableBorderDxfId="156" totalsRowBorderDxfId="155">
-  <autoFilter ref="A1:O5"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table24" displayName="Table24" ref="A1:P5" totalsRowShown="0" headerRowDxfId="168" dataDxfId="166" headerRowBorderDxfId="167" tableBorderDxfId="165" totalsRowBorderDxfId="164">
+  <autoFilter ref="A1:P5"/>
   <sortState ref="A2:O38">
     <sortCondition ref="L1:L38"/>
   </sortState>
-  <tableColumns count="15">
-    <tableColumn id="1" name="Description" dataDxfId="154"/>
-    <tableColumn id="16" name="ExecutionPipeLine" dataDxfId="153"/>
-    <tableColumn id="17" name="CheckInDate" dataDxfId="152"/>
-    <tableColumn id="18" name="CheckOutDate" dataDxfId="151"/>
-    <tableColumn id="3" name="ShortLocation" dataDxfId="150"/>
-    <tableColumn id="4" name="Location" dataDxfId="149"/>
-    <tableColumn id="5" name="Adults" dataDxfId="148"/>
-    <tableColumn id="6" name="ChildrenAges" dataDxfId="147"/>
-    <tableColumn id="8" name="AdditionalPreferences" dataDxfId="146"/>
-    <tableColumn id="9" name="HotelName" dataDxfId="145"/>
-    <tableColumn id="10" name="StarRating" dataDxfId="144"/>
-    <tableColumn id="11" name="Supplier" dataDxfId="143"/>
-    <tableColumn id="7" name="UserType" dataDxfId="142"/>
-    <tableColumn id="14" name="PostSearchFilters" dataDxfId="141"/>
-    <tableColumn id="15" name="PostSearchFilterValues" dataDxfId="140"/>
+  <tableColumns count="16">
+    <tableColumn id="1" name="Description" dataDxfId="163"/>
+    <tableColumn id="16" name="ExecutionPipeLine" dataDxfId="162"/>
+    <tableColumn id="17" name="CheckInDate" dataDxfId="161"/>
+    <tableColumn id="18" name="CheckOutDate" dataDxfId="160"/>
+    <tableColumn id="3" name="ShortLocation" dataDxfId="159"/>
+    <tableColumn id="4" name="Location" dataDxfId="158"/>
+    <tableColumn id="5" name="Adults" dataDxfId="157"/>
+    <tableColumn id="6" name="ChildrenAges" dataDxfId="156"/>
+    <tableColumn id="8" name="AdditionalPreferences" dataDxfId="155"/>
+    <tableColumn id="9" name="HotelName" dataDxfId="154"/>
+    <tableColumn id="10" name="StarRating" dataDxfId="153"/>
+    <tableColumn id="11" name="Supplier" dataDxfId="152"/>
+    <tableColumn id="7" name="UserType" dataDxfId="151"/>
+    <tableColumn id="2" name="PaymentMode" dataDxfId="8"/>
+    <tableColumn id="14" name="PostSearchFilters" dataDxfId="150"/>
+    <tableColumn id="15" name="PostSearchFilterValues" dataDxfId="149"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Table25" displayName="Table25" ref="A1:O3" totalsRowShown="0" headerRowDxfId="139" dataDxfId="137" headerRowBorderDxfId="138" tableBorderDxfId="136" totalsRowBorderDxfId="135">
-  <autoFilter ref="A1:O3"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Table25" displayName="Table25" ref="A1:P3" totalsRowShown="0" headerRowDxfId="148" dataDxfId="146" headerRowBorderDxfId="147" tableBorderDxfId="145" totalsRowBorderDxfId="144">
+  <autoFilter ref="A1:P3"/>
   <sortState ref="A2:O38">
     <sortCondition ref="L1:L38"/>
   </sortState>
-  <tableColumns count="15">
-    <tableColumn id="1" name="Description" dataDxfId="134"/>
-    <tableColumn id="16" name="ExecutionPipeLine" dataDxfId="133"/>
-    <tableColumn id="17" name="CheckInDate" dataDxfId="132"/>
-    <tableColumn id="18" name="CheckOutDate" dataDxfId="131"/>
-    <tableColumn id="3" name="ShortLocation" dataDxfId="130"/>
-    <tableColumn id="4" name="Location" dataDxfId="129"/>
-    <tableColumn id="5" name="Adults" dataDxfId="128"/>
-    <tableColumn id="6" name="ChildrenAges" dataDxfId="127"/>
-    <tableColumn id="8" name="AdditionalPreferences" dataDxfId="126"/>
-    <tableColumn id="9" name="HotelName" dataDxfId="125"/>
-    <tableColumn id="10" name="StarRating" dataDxfId="124"/>
-    <tableColumn id="11" name="Supplier" dataDxfId="123"/>
-    <tableColumn id="7" name="UserType" dataDxfId="122"/>
-    <tableColumn id="14" name="PostSearchFilters" dataDxfId="121"/>
-    <tableColumn id="15" name="PostSearchFilterValues" dataDxfId="120"/>
+  <tableColumns count="16">
+    <tableColumn id="1" name="Description" dataDxfId="143"/>
+    <tableColumn id="16" name="ExecutionPipeLine" dataDxfId="142"/>
+    <tableColumn id="17" name="CheckInDate" dataDxfId="141"/>
+    <tableColumn id="18" name="CheckOutDate" dataDxfId="140"/>
+    <tableColumn id="3" name="ShortLocation" dataDxfId="139"/>
+    <tableColumn id="4" name="Location" dataDxfId="138"/>
+    <tableColumn id="5" name="Adults" dataDxfId="137"/>
+    <tableColumn id="6" name="ChildrenAges" dataDxfId="136"/>
+    <tableColumn id="8" name="AdditionalPreferences" dataDxfId="135"/>
+    <tableColumn id="9" name="HotelName" dataDxfId="134"/>
+    <tableColumn id="10" name="StarRating" dataDxfId="133"/>
+    <tableColumn id="11" name="Supplier" dataDxfId="132"/>
+    <tableColumn id="7" name="UserType" dataDxfId="131"/>
+    <tableColumn id="2" name="PaymentMode" dataDxfId="5"/>
+    <tableColumn id="14" name="PostSearchFilters" dataDxfId="130"/>
+    <tableColumn id="15" name="PostSearchFilterValues" dataDxfId="129"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Table26" displayName="Table26" ref="A1:O4" totalsRowShown="0" headerRowDxfId="119" dataDxfId="117" headerRowBorderDxfId="118" tableBorderDxfId="116" totalsRowBorderDxfId="115">
-  <autoFilter ref="A1:O4"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Table26" displayName="Table26" ref="A1:P4" totalsRowShown="0" headerRowDxfId="128" dataDxfId="126" headerRowBorderDxfId="127" tableBorderDxfId="125" totalsRowBorderDxfId="124">
+  <autoFilter ref="A1:P4"/>
   <sortState ref="A2:O38">
     <sortCondition ref="L1:L38"/>
   </sortState>
-  <tableColumns count="15">
-    <tableColumn id="1" name="Description" dataDxfId="114"/>
-    <tableColumn id="16" name="ExecutionPipeLine" dataDxfId="113"/>
-    <tableColumn id="17" name="CheckInDate" dataDxfId="112"/>
-    <tableColumn id="18" name="CheckOutDate" dataDxfId="111"/>
-    <tableColumn id="3" name="ShortLocation" dataDxfId="110"/>
-    <tableColumn id="4" name="Location" dataDxfId="109"/>
-    <tableColumn id="5" name="Adults" dataDxfId="108"/>
-    <tableColumn id="6" name="ChildrenAges" dataDxfId="107"/>
-    <tableColumn id="8" name="AdditionalPreferences" dataDxfId="106"/>
-    <tableColumn id="9" name="HotelName" dataDxfId="105"/>
-    <tableColumn id="10" name="StarRating" dataDxfId="104"/>
-    <tableColumn id="11" name="Supplier" dataDxfId="103"/>
-    <tableColumn id="7" name="UserType" dataDxfId="102"/>
-    <tableColumn id="14" name="PostSearchFilters" dataDxfId="101"/>
-    <tableColumn id="15" name="PostSearchFilterValues" dataDxfId="100"/>
+  <tableColumns count="16">
+    <tableColumn id="1" name="Description" dataDxfId="123"/>
+    <tableColumn id="16" name="ExecutionPipeLine" dataDxfId="122"/>
+    <tableColumn id="17" name="CheckInDate" dataDxfId="121"/>
+    <tableColumn id="18" name="CheckOutDate" dataDxfId="120"/>
+    <tableColumn id="3" name="ShortLocation" dataDxfId="119"/>
+    <tableColumn id="4" name="Location" dataDxfId="118"/>
+    <tableColumn id="5" name="Adults" dataDxfId="117"/>
+    <tableColumn id="6" name="ChildrenAges" dataDxfId="116"/>
+    <tableColumn id="8" name="AdditionalPreferences" dataDxfId="115"/>
+    <tableColumn id="9" name="HotelName" dataDxfId="114"/>
+    <tableColumn id="10" name="StarRating" dataDxfId="113"/>
+    <tableColumn id="11" name="Supplier" dataDxfId="112"/>
+    <tableColumn id="7" name="UserType" dataDxfId="111"/>
+    <tableColumn id="2" name="PaymentMode" dataDxfId="4"/>
+    <tableColumn id="14" name="PostSearchFilters" dataDxfId="110"/>
+    <tableColumn id="15" name="PostSearchFilterValues" dataDxfId="109"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="Table27" displayName="Table27" ref="A1:O3" totalsRowShown="0" headerRowDxfId="99" dataDxfId="97" headerRowBorderDxfId="98" tableBorderDxfId="96" totalsRowBorderDxfId="95">
-  <autoFilter ref="A1:O3"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="Table27" displayName="Table27" ref="A1:P3" totalsRowShown="0" headerRowDxfId="108" dataDxfId="106" headerRowBorderDxfId="107" tableBorderDxfId="105" totalsRowBorderDxfId="104">
+  <autoFilter ref="A1:P3"/>
   <sortState ref="A2:O38">
     <sortCondition ref="L1:L38"/>
   </sortState>
-  <tableColumns count="15">
-    <tableColumn id="1" name="Description" dataDxfId="94"/>
-    <tableColumn id="16" name="ExecutionPipeLine" dataDxfId="93"/>
-    <tableColumn id="17" name="CheckInDate" dataDxfId="92"/>
-    <tableColumn id="18" name="CheckOutDate" dataDxfId="91"/>
-    <tableColumn id="3" name="ShortLocation" dataDxfId="90"/>
-    <tableColumn id="4" name="Location" dataDxfId="89"/>
-    <tableColumn id="5" name="Adults" dataDxfId="88"/>
-    <tableColumn id="6" name="ChildrenAges" dataDxfId="87"/>
-    <tableColumn id="8" name="AdditionalPreferences" dataDxfId="86"/>
-    <tableColumn id="9" name="HotelName" dataDxfId="85"/>
-    <tableColumn id="10" name="StarRating" dataDxfId="84"/>
-    <tableColumn id="11" name="Supplier" dataDxfId="83"/>
-    <tableColumn id="7" name="UserType" dataDxfId="82"/>
-    <tableColumn id="14" name="PostSearchFilters" dataDxfId="81"/>
-    <tableColumn id="15" name="PostSearchFilterValues" dataDxfId="80"/>
+  <tableColumns count="16">
+    <tableColumn id="1" name="Description" dataDxfId="103"/>
+    <tableColumn id="16" name="ExecutionPipeLine" dataDxfId="102"/>
+    <tableColumn id="17" name="CheckInDate" dataDxfId="101"/>
+    <tableColumn id="18" name="CheckOutDate" dataDxfId="100"/>
+    <tableColumn id="3" name="ShortLocation" dataDxfId="99"/>
+    <tableColumn id="4" name="Location" dataDxfId="98"/>
+    <tableColumn id="5" name="Adults" dataDxfId="97"/>
+    <tableColumn id="6" name="ChildrenAges" dataDxfId="96"/>
+    <tableColumn id="8" name="AdditionalPreferences" dataDxfId="95"/>
+    <tableColumn id="9" name="HotelName" dataDxfId="94"/>
+    <tableColumn id="10" name="StarRating" dataDxfId="93"/>
+    <tableColumn id="11" name="Supplier" dataDxfId="92"/>
+    <tableColumn id="7" name="UserType" dataDxfId="91"/>
+    <tableColumn id="2" name="PaymentMode" dataDxfId="3"/>
+    <tableColumn id="14" name="PostSearchFilters" dataDxfId="90"/>
+    <tableColumn id="15" name="PostSearchFilterValues" dataDxfId="89"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="7" name="Table28" displayName="Table28" ref="A1:O4" totalsRowShown="0" headerRowDxfId="79" dataDxfId="77" headerRowBorderDxfId="78" tableBorderDxfId="76" totalsRowBorderDxfId="75">
-  <autoFilter ref="A1:O4"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="7" name="Table28" displayName="Table28" ref="A1:P4" totalsRowShown="0" headerRowDxfId="88" dataDxfId="86" headerRowBorderDxfId="87" tableBorderDxfId="85" totalsRowBorderDxfId="84">
+  <autoFilter ref="A1:P4"/>
   <sortState ref="A2:O38">
     <sortCondition ref="L1:L38"/>
   </sortState>
-  <tableColumns count="15">
-    <tableColumn id="1" name="Description" dataDxfId="74"/>
-    <tableColumn id="16" name="ExecutionPipeLine" dataDxfId="73"/>
-    <tableColumn id="17" name="CheckInDate" dataDxfId="72"/>
-    <tableColumn id="18" name="CheckOutDate" dataDxfId="71"/>
-    <tableColumn id="3" name="ShortLocation" dataDxfId="70"/>
-    <tableColumn id="4" name="Location" dataDxfId="69"/>
-    <tableColumn id="5" name="Adults" dataDxfId="68"/>
-    <tableColumn id="6" name="ChildrenAges" dataDxfId="67"/>
-    <tableColumn id="8" name="AdditionalPreferences" dataDxfId="66"/>
-    <tableColumn id="9" name="HotelName" dataDxfId="65"/>
-    <tableColumn id="10" name="StarRating" dataDxfId="64"/>
-    <tableColumn id="11" name="Supplier" dataDxfId="63"/>
-    <tableColumn id="7" name="UserType" dataDxfId="62"/>
-    <tableColumn id="14" name="PostSearchFilters" dataDxfId="61"/>
-    <tableColumn id="15" name="PostSearchFilterValues" dataDxfId="60"/>
+  <tableColumns count="16">
+    <tableColumn id="1" name="Description" dataDxfId="83"/>
+    <tableColumn id="16" name="ExecutionPipeLine" dataDxfId="82"/>
+    <tableColumn id="17" name="CheckInDate" dataDxfId="81"/>
+    <tableColumn id="18" name="CheckOutDate" dataDxfId="80"/>
+    <tableColumn id="3" name="ShortLocation" dataDxfId="79"/>
+    <tableColumn id="4" name="Location" dataDxfId="78"/>
+    <tableColumn id="5" name="Adults" dataDxfId="77"/>
+    <tableColumn id="6" name="ChildrenAges" dataDxfId="76"/>
+    <tableColumn id="8" name="AdditionalPreferences" dataDxfId="75"/>
+    <tableColumn id="9" name="HotelName" dataDxfId="74"/>
+    <tableColumn id="10" name="StarRating" dataDxfId="73"/>
+    <tableColumn id="11" name="Supplier" dataDxfId="72"/>
+    <tableColumn id="7" name="UserType" dataDxfId="71"/>
+    <tableColumn id="2" name="PaymentMode" dataDxfId="2"/>
+    <tableColumn id="14" name="PostSearchFilters" dataDxfId="70"/>
+    <tableColumn id="15" name="PostSearchFilterValues" dataDxfId="69"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="8" name="Table29" displayName="Table29" ref="A1:O7" totalsRowShown="0" headerRowDxfId="59" dataDxfId="57" headerRowBorderDxfId="58" tableBorderDxfId="56" totalsRowBorderDxfId="55">
-  <autoFilter ref="A1:O7"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="8" name="Table29" displayName="Table29" ref="A1:P7" totalsRowShown="0" headerRowDxfId="68" dataDxfId="66" headerRowBorderDxfId="67" tableBorderDxfId="65" totalsRowBorderDxfId="64">
+  <autoFilter ref="A1:P7"/>
   <sortState ref="A2:O38">
     <sortCondition ref="L1:L38"/>
   </sortState>
-  <tableColumns count="15">
-    <tableColumn id="1" name="Description" dataDxfId="54"/>
-    <tableColumn id="16" name="ExecutionPipeLine" dataDxfId="53"/>
-    <tableColumn id="17" name="CheckInDate" dataDxfId="52"/>
-    <tableColumn id="18" name="CheckOutDate" dataDxfId="51"/>
-    <tableColumn id="3" name="ShortLocation" dataDxfId="50"/>
-    <tableColumn id="4" name="Location" dataDxfId="49"/>
-    <tableColumn id="5" name="Adults" dataDxfId="48"/>
-    <tableColumn id="6" name="ChildrenAges" dataDxfId="47"/>
-    <tableColumn id="8" name="AdditionalPreferences" dataDxfId="46"/>
-    <tableColumn id="9" name="HotelName" dataDxfId="45"/>
-    <tableColumn id="10" name="StarRating" dataDxfId="44"/>
-    <tableColumn id="11" name="Supplier" dataDxfId="43"/>
-    <tableColumn id="7" name="UserType" dataDxfId="42"/>
-    <tableColumn id="14" name="PostSearchFilters" dataDxfId="41"/>
-    <tableColumn id="15" name="PostSearchFilterValues" dataDxfId="40"/>
+  <tableColumns count="16">
+    <tableColumn id="1" name="Description" dataDxfId="63"/>
+    <tableColumn id="16" name="ExecutionPipeLine" dataDxfId="62"/>
+    <tableColumn id="17" name="CheckInDate" dataDxfId="61"/>
+    <tableColumn id="18" name="CheckOutDate" dataDxfId="60"/>
+    <tableColumn id="3" name="ShortLocation" dataDxfId="59"/>
+    <tableColumn id="4" name="Location" dataDxfId="58"/>
+    <tableColumn id="5" name="Adults" dataDxfId="57"/>
+    <tableColumn id="6" name="ChildrenAges" dataDxfId="56"/>
+    <tableColumn id="8" name="AdditionalPreferences" dataDxfId="55"/>
+    <tableColumn id="9" name="HotelName" dataDxfId="54"/>
+    <tableColumn id="10" name="StarRating" dataDxfId="53"/>
+    <tableColumn id="11" name="Supplier" dataDxfId="52"/>
+    <tableColumn id="7" name="UserType" dataDxfId="51"/>
+    <tableColumn id="2" name="PaymentMode" dataDxfId="1"/>
+    <tableColumn id="14" name="PostSearchFilters" dataDxfId="50"/>
+    <tableColumn id="15" name="PostSearchFilterValues" dataDxfId="49"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table9.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="9" name="Table2101110" displayName="Table2101110" ref="A1:O17" totalsRowShown="0" headerRowDxfId="19" dataDxfId="18" headerRowBorderDxfId="16" tableBorderDxfId="17" totalsRowBorderDxfId="15">
-  <autoFilter ref="A1:O17"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="9" name="Table2101110" displayName="Table2101110" ref="A1:P17" totalsRowShown="0" headerRowDxfId="48" dataDxfId="46" headerRowBorderDxfId="47" tableBorderDxfId="45" totalsRowBorderDxfId="44">
+  <autoFilter ref="A1:P17"/>
   <sortState ref="A2:O38">
     <sortCondition ref="L1:L38"/>
   </sortState>
-  <tableColumns count="15">
-    <tableColumn id="1" name="Description" dataDxfId="14"/>
-    <tableColumn id="16" name="ExecutionPipeLine" dataDxfId="13"/>
-    <tableColumn id="17" name="CheckInDate" dataDxfId="12"/>
-    <tableColumn id="18" name="CheckOutDate" dataDxfId="11"/>
-    <tableColumn id="3" name="ShortLocation" dataDxfId="10"/>
-    <tableColumn id="4" name="Location" dataDxfId="9"/>
-    <tableColumn id="5" name="Adults" dataDxfId="8"/>
-    <tableColumn id="6" name="ChildrenAges" dataDxfId="7"/>
-    <tableColumn id="8" name="AdditionalPreferences" dataDxfId="6"/>
-    <tableColumn id="9" name="HotelName" dataDxfId="5"/>
-    <tableColumn id="10" name="StarRating" dataDxfId="4"/>
-    <tableColumn id="11" name="Supplier" dataDxfId="3"/>
-    <tableColumn id="7" name="UserType" dataDxfId="2"/>
-    <tableColumn id="14" name="PostSearchFilters" dataDxfId="1"/>
-    <tableColumn id="15" name="PostSearchFilterValues" dataDxfId="0"/>
+  <tableColumns count="16">
+    <tableColumn id="1" name="Description" dataDxfId="43"/>
+    <tableColumn id="16" name="ExecutionPipeLine" dataDxfId="42"/>
+    <tableColumn id="17" name="CheckInDate" dataDxfId="41"/>
+    <tableColumn id="18" name="CheckOutDate" dataDxfId="40"/>
+    <tableColumn id="3" name="ShortLocation" dataDxfId="39"/>
+    <tableColumn id="4" name="Location" dataDxfId="38"/>
+    <tableColumn id="5" name="Adults" dataDxfId="37"/>
+    <tableColumn id="6" name="ChildrenAges" dataDxfId="36"/>
+    <tableColumn id="8" name="AdditionalPreferences" dataDxfId="35"/>
+    <tableColumn id="9" name="HotelName" dataDxfId="34"/>
+    <tableColumn id="10" name="StarRating" dataDxfId="33"/>
+    <tableColumn id="11" name="Supplier" dataDxfId="32"/>
+    <tableColumn id="7" name="UserType" dataDxfId="31"/>
+    <tableColumn id="2" name="PaymentMode" dataDxfId="0"/>
+    <tableColumn id="14" name="PostSearchFilters" dataDxfId="30"/>
+    <tableColumn id="15" name="PostSearchFilterValues" dataDxfId="29"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -4247,12 +4382,12 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O38"/>
+  <dimension ref="A1:P38"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="1" topLeftCell="D1" activePane="topRight" state="frozen"/>
+    <sheetView topLeftCell="A19" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="G1" activePane="topRight" state="frozen"/>
       <selection activeCell="A4" sqref="A4"/>
-      <selection pane="topRight" activeCell="J3" sqref="J3"/>
+      <selection pane="topRight" activeCell="N1" sqref="N1:N38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4268,12 +4403,12 @@
     <col min="10" max="10" width="36.7109375" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="16.140625" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="18" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="18" customWidth="1"/>
-    <col min="14" max="14" width="22.28515625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="20.5703125" bestFit="1" customWidth="1"/>
+    <col min="13" max="14" width="18" customWidth="1"/>
+    <col min="15" max="15" width="22.28515625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="20.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -4314,13 +4449,16 @@
         <v>15</v>
       </c>
       <c r="N1" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="O1" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="O1" s="3" t="s">
+      <c r="P1" s="3" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:15" ht="30" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:16" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="12" t="s">
         <v>88</v>
       </c>
@@ -4352,10 +4490,13 @@
       <c r="M2" s="9" t="s">
         <v>38</v>
       </c>
-      <c r="N2" s="5"/>
-      <c r="O2" s="17"/>
-    </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="N2" s="5" t="s">
+        <v>105</v>
+      </c>
+      <c r="O2" s="5"/>
+      <c r="P2" s="17"/>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A3" s="12" t="s">
         <v>20</v>
       </c>
@@ -4389,10 +4530,13 @@
       <c r="M3" s="9" t="s">
         <v>39</v>
       </c>
-      <c r="N3" s="5"/>
-      <c r="O3" s="17"/>
-    </row>
-    <row r="4" spans="1:15" ht="30" x14ac:dyDescent="0.25">
+      <c r="N3" s="5" t="s">
+        <v>105</v>
+      </c>
+      <c r="O3" s="5"/>
+      <c r="P3" s="17"/>
+    </row>
+    <row r="4" spans="1:16" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" s="12" t="s">
         <v>87</v>
       </c>
@@ -4424,10 +4568,13 @@
       <c r="M4" s="9" t="s">
         <v>39</v>
       </c>
-      <c r="N4" s="5"/>
-      <c r="O4" s="17"/>
-    </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="N4" s="5" t="s">
+        <v>105</v>
+      </c>
+      <c r="O4" s="5"/>
+      <c r="P4" s="17"/>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A5" s="12" t="s">
         <v>16</v>
       </c>
@@ -4459,10 +4606,13 @@
       <c r="M5" s="9" t="s">
         <v>38</v>
       </c>
-      <c r="N5" s="5"/>
-      <c r="O5" s="17"/>
-    </row>
-    <row r="6" spans="1:15" ht="30" x14ac:dyDescent="0.25">
+      <c r="N5" s="5" t="s">
+        <v>105</v>
+      </c>
+      <c r="O5" s="5"/>
+      <c r="P5" s="17"/>
+    </row>
+    <row r="6" spans="1:16" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" s="12" t="s">
         <v>19</v>
       </c>
@@ -4500,10 +4650,13 @@
       <c r="M6" s="9" t="s">
         <v>38</v>
       </c>
-      <c r="N6" s="5"/>
-      <c r="O6" s="17"/>
-    </row>
-    <row r="7" spans="1:15" ht="30" x14ac:dyDescent="0.25">
+      <c r="N6" s="5" t="s">
+        <v>105</v>
+      </c>
+      <c r="O6" s="5"/>
+      <c r="P6" s="17"/>
+    </row>
+    <row r="7" spans="1:16" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" s="12" t="s">
         <v>22</v>
       </c>
@@ -4539,10 +4692,13 @@
       <c r="M7" s="9" t="s">
         <v>39</v>
       </c>
-      <c r="N7" s="5"/>
-      <c r="O7" s="17"/>
-    </row>
-    <row r="8" spans="1:15" ht="30" x14ac:dyDescent="0.25">
+      <c r="N7" s="5" t="s">
+        <v>105</v>
+      </c>
+      <c r="O7" s="5"/>
+      <c r="P7" s="17"/>
+    </row>
+    <row r="8" spans="1:16" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" s="12" t="s">
         <v>91</v>
       </c>
@@ -4576,10 +4732,13 @@
       <c r="M8" s="9" t="s">
         <v>38</v>
       </c>
-      <c r="N8" s="5"/>
-      <c r="O8" s="17"/>
-    </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="N8" s="5" t="s">
+        <v>105</v>
+      </c>
+      <c r="O8" s="5"/>
+      <c r="P8" s="17"/>
+    </row>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A9" s="12" t="s">
         <v>18</v>
       </c>
@@ -4613,10 +4772,13 @@
       <c r="M9" s="9" t="s">
         <v>39</v>
       </c>
-      <c r="N9" s="5"/>
-      <c r="O9" s="17"/>
-    </row>
-    <row r="10" spans="1:15" ht="30" x14ac:dyDescent="0.25">
+      <c r="N9" s="5" t="s">
+        <v>105</v>
+      </c>
+      <c r="O9" s="5"/>
+      <c r="P9" s="17"/>
+    </row>
+    <row r="10" spans="1:16" ht="30" x14ac:dyDescent="0.25">
       <c r="A10" s="12" t="s">
         <v>89</v>
       </c>
@@ -4648,10 +4810,13 @@
       <c r="M10" s="9" t="s">
         <v>38</v>
       </c>
-      <c r="N10" s="5"/>
-      <c r="O10" s="17"/>
-    </row>
-    <row r="11" spans="1:15" ht="30" x14ac:dyDescent="0.25">
+      <c r="N10" s="5" t="s">
+        <v>105</v>
+      </c>
+      <c r="O10" s="5"/>
+      <c r="P10" s="17"/>
+    </row>
+    <row r="11" spans="1:16" ht="30" x14ac:dyDescent="0.25">
       <c r="A11" s="12" t="s">
         <v>90</v>
       </c>
@@ -4685,10 +4850,13 @@
       <c r="M11" s="9" t="s">
         <v>38</v>
       </c>
-      <c r="N11" s="5"/>
-      <c r="O11" s="17"/>
-    </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="N11" s="5" t="s">
+        <v>105</v>
+      </c>
+      <c r="O11" s="5"/>
+      <c r="P11" s="17"/>
+    </row>
+    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A12" s="12" t="s">
         <v>17</v>
       </c>
@@ -4724,10 +4892,13 @@
       <c r="M12" s="9" t="s">
         <v>39</v>
       </c>
-      <c r="N12" s="5"/>
-      <c r="O12" s="17"/>
-    </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="N12" s="5" t="s">
+        <v>105</v>
+      </c>
+      <c r="O12" s="5"/>
+      <c r="P12" s="17"/>
+    </row>
+    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A13" s="12" t="s">
         <v>41</v>
       </c>
@@ -4765,10 +4936,13 @@
       <c r="M13" s="9" t="s">
         <v>39</v>
       </c>
-      <c r="N13" s="5"/>
-      <c r="O13" s="17"/>
-    </row>
-    <row r="14" spans="1:15" ht="30" x14ac:dyDescent="0.25">
+      <c r="N13" s="5" t="s">
+        <v>105</v>
+      </c>
+      <c r="O13" s="5"/>
+      <c r="P13" s="17"/>
+    </row>
+    <row r="14" spans="1:16" ht="30" x14ac:dyDescent="0.25">
       <c r="A14" s="12" t="s">
         <v>23</v>
       </c>
@@ -4800,10 +4974,13 @@
       <c r="M14" s="9" t="s">
         <v>39</v>
       </c>
-      <c r="N14" s="5"/>
-      <c r="O14" s="17"/>
-    </row>
-    <row r="15" spans="1:15" ht="30" x14ac:dyDescent="0.25">
+      <c r="N14" s="5" t="s">
+        <v>105</v>
+      </c>
+      <c r="O14" s="5"/>
+      <c r="P14" s="17"/>
+    </row>
+    <row r="15" spans="1:16" ht="30" x14ac:dyDescent="0.25">
       <c r="A15" s="12" t="s">
         <v>50</v>
       </c>
@@ -4837,10 +5014,13 @@
       <c r="M15" s="9" t="s">
         <v>39</v>
       </c>
-      <c r="N15" s="5"/>
-      <c r="O15" s="17"/>
-    </row>
-    <row r="16" spans="1:15" ht="30" x14ac:dyDescent="0.25">
+      <c r="N15" s="5" t="s">
+        <v>105</v>
+      </c>
+      <c r="O15" s="5"/>
+      <c r="P15" s="17"/>
+    </row>
+    <row r="16" spans="1:16" ht="30" x14ac:dyDescent="0.25">
       <c r="A16" s="12" t="s">
         <v>92</v>
       </c>
@@ -4874,10 +5054,13 @@
       <c r="M16" s="9" t="s">
         <v>38</v>
       </c>
-      <c r="N16" s="5"/>
-      <c r="O16" s="17"/>
-    </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="N16" s="5" t="s">
+        <v>105</v>
+      </c>
+      <c r="O16" s="5"/>
+      <c r="P16" s="17"/>
+    </row>
+    <row r="17" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A17" s="12" t="s">
         <v>21</v>
       </c>
@@ -4911,10 +5094,13 @@
       <c r="M17" s="9" t="s">
         <v>39</v>
       </c>
-      <c r="N17" s="5"/>
-      <c r="O17" s="17"/>
-    </row>
-    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="N17" s="5" t="s">
+        <v>105</v>
+      </c>
+      <c r="O17" s="5"/>
+      <c r="P17" s="17"/>
+    </row>
+    <row r="18" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A18" s="12" t="s">
         <v>42</v>
       </c>
@@ -4950,10 +5136,13 @@
       <c r="M18" s="9" t="s">
         <v>39</v>
       </c>
-      <c r="N18" s="5"/>
-      <c r="O18" s="17"/>
-    </row>
-    <row r="19" spans="1:15" ht="30" x14ac:dyDescent="0.25">
+      <c r="N18" s="5" t="s">
+        <v>105</v>
+      </c>
+      <c r="O18" s="5"/>
+      <c r="P18" s="17"/>
+    </row>
+    <row r="19" spans="1:16" ht="30" x14ac:dyDescent="0.25">
       <c r="A19" s="12" t="s">
         <v>43</v>
       </c>
@@ -4991,10 +5180,13 @@
       <c r="M19" s="9" t="s">
         <v>39</v>
       </c>
-      <c r="N19" s="5"/>
-      <c r="O19" s="17"/>
-    </row>
-    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="N19" s="5" t="s">
+        <v>105</v>
+      </c>
+      <c r="O19" s="5"/>
+      <c r="P19" s="17"/>
+    </row>
+    <row r="20" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A20" s="12" t="s">
         <v>44</v>
       </c>
@@ -5030,10 +5222,13 @@
       <c r="M20" s="9" t="s">
         <v>39</v>
       </c>
-      <c r="N20" s="5"/>
-      <c r="O20" s="17"/>
-    </row>
-    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="N20" s="5" t="s">
+        <v>105</v>
+      </c>
+      <c r="O20" s="5"/>
+      <c r="P20" s="17"/>
+    </row>
+    <row r="21" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A21" s="12" t="s">
         <v>24</v>
       </c>
@@ -5067,10 +5262,13 @@
       <c r="M21" s="9" t="s">
         <v>39</v>
       </c>
-      <c r="N21" s="5"/>
-      <c r="O21" s="17"/>
-    </row>
-    <row r="22" spans="1:15" ht="30" x14ac:dyDescent="0.25">
+      <c r="N21" s="5" t="s">
+        <v>105</v>
+      </c>
+      <c r="O21" s="5"/>
+      <c r="P21" s="17"/>
+    </row>
+    <row r="22" spans="1:16" ht="30" x14ac:dyDescent="0.25">
       <c r="A22" s="12" t="s">
         <v>51</v>
       </c>
@@ -5106,10 +5304,13 @@
       <c r="M22" s="9" t="s">
         <v>39</v>
       </c>
-      <c r="N22" s="5"/>
-      <c r="O22" s="17"/>
-    </row>
-    <row r="23" spans="1:15" ht="30" x14ac:dyDescent="0.25">
+      <c r="N22" s="5" t="s">
+        <v>105</v>
+      </c>
+      <c r="O22" s="5"/>
+      <c r="P22" s="17"/>
+    </row>
+    <row r="23" spans="1:16" ht="30" x14ac:dyDescent="0.25">
       <c r="A23" s="13" t="s">
         <v>25</v>
       </c>
@@ -5141,10 +5342,13 @@
       <c r="M23" s="9" t="s">
         <v>39</v>
       </c>
-      <c r="N23" s="5"/>
-      <c r="O23" s="17"/>
-    </row>
-    <row r="24" spans="1:15" ht="30" x14ac:dyDescent="0.25">
+      <c r="N23" s="5" t="s">
+        <v>105</v>
+      </c>
+      <c r="O23" s="5"/>
+      <c r="P23" s="17"/>
+    </row>
+    <row r="24" spans="1:16" ht="30" x14ac:dyDescent="0.25">
       <c r="A24" s="13" t="s">
         <v>26</v>
       </c>
@@ -5175,13 +5379,16 @@
         <v>38</v>
       </c>
       <c r="N24" s="5" t="s">
+        <v>105</v>
+      </c>
+      <c r="O24" s="5" t="s">
         <v>74</v>
       </c>
-      <c r="O24" s="6" t="s">
+      <c r="P24" s="6" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="25" spans="1:15" ht="30" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:16" ht="30" x14ac:dyDescent="0.25">
       <c r="A25" s="13" t="s">
         <v>27</v>
       </c>
@@ -5214,13 +5421,16 @@
         <v>39</v>
       </c>
       <c r="N25" s="5" t="s">
+        <v>105</v>
+      </c>
+      <c r="O25" s="5" t="s">
         <v>72</v>
       </c>
-      <c r="O25" s="17" t="s">
+      <c r="P25" s="17" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="26" spans="1:15" ht="30" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:16" ht="30" x14ac:dyDescent="0.25">
       <c r="A26" s="14" t="s">
         <v>28</v>
       </c>
@@ -5252,10 +5462,13 @@
       <c r="M26" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="N26" s="5"/>
-      <c r="O26" s="17"/>
-    </row>
-    <row r="27" spans="1:15" ht="30" x14ac:dyDescent="0.25">
+      <c r="N26" s="5" t="s">
+        <v>105</v>
+      </c>
+      <c r="O26" s="5"/>
+      <c r="P26" s="17"/>
+    </row>
+    <row r="27" spans="1:16" ht="30" x14ac:dyDescent="0.25">
       <c r="A27" s="14" t="s">
         <v>29</v>
       </c>
@@ -5286,13 +5499,16 @@
         <v>39</v>
       </c>
       <c r="N27" s="5" t="s">
+        <v>105</v>
+      </c>
+      <c r="O27" s="5" t="s">
         <v>76</v>
       </c>
-      <c r="O27" s="11" t="s">
+      <c r="P27" s="11" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="28" spans="1:15" ht="30" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:16" ht="30" x14ac:dyDescent="0.25">
       <c r="A28" s="13" t="s">
         <v>30</v>
       </c>
@@ -5323,13 +5539,16 @@
         <v>39</v>
       </c>
       <c r="N28" s="5" t="s">
+        <v>105</v>
+      </c>
+      <c r="O28" s="5" t="s">
         <v>77</v>
       </c>
-      <c r="O28" s="10" t="s">
+      <c r="P28" s="10" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="29" spans="1:15" ht="30" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:16" ht="30" x14ac:dyDescent="0.25">
       <c r="A29" s="13" t="s">
         <v>31</v>
       </c>
@@ -5360,13 +5579,16 @@
         <v>39</v>
       </c>
       <c r="N29" s="5" t="s">
+        <v>105</v>
+      </c>
+      <c r="O29" s="5" t="s">
         <v>77</v>
       </c>
-      <c r="O29" s="10" t="s">
+      <c r="P29" s="10" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="30" spans="1:15" ht="30" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:16" ht="30" x14ac:dyDescent="0.25">
       <c r="A30" s="13" t="s">
         <v>32</v>
       </c>
@@ -5397,13 +5619,16 @@
         <v>39</v>
       </c>
       <c r="N30" s="5" t="s">
+        <v>105</v>
+      </c>
+      <c r="O30" s="5" t="s">
         <v>77</v>
       </c>
-      <c r="O30" s="10" t="s">
+      <c r="P30" s="10" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="31" spans="1:15" ht="30" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:16" ht="30" x14ac:dyDescent="0.25">
       <c r="A31" s="13" t="s">
         <v>33</v>
       </c>
@@ -5434,13 +5659,16 @@
         <v>39</v>
       </c>
       <c r="N31" s="5" t="s">
+        <v>105</v>
+      </c>
+      <c r="O31" s="5" t="s">
         <v>77</v>
       </c>
-      <c r="O31" s="10" t="s">
+      <c r="P31" s="10" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="32" spans="1:15" ht="30" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:16" ht="30" x14ac:dyDescent="0.25">
       <c r="A32" s="13" t="s">
         <v>34</v>
       </c>
@@ -5471,13 +5699,16 @@
         <v>39</v>
       </c>
       <c r="N32" s="5" t="s">
+        <v>105</v>
+      </c>
+      <c r="O32" s="5" t="s">
         <v>77</v>
       </c>
-      <c r="O32" s="10" t="s">
+      <c r="P32" s="10" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="33" spans="1:15" ht="30" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:16" ht="30" x14ac:dyDescent="0.25">
       <c r="A33" s="13" t="s">
         <v>35</v>
       </c>
@@ -5508,13 +5739,16 @@
         <v>39</v>
       </c>
       <c r="N33" s="5" t="s">
+        <v>105</v>
+      </c>
+      <c r="O33" s="5" t="s">
         <v>77</v>
       </c>
-      <c r="O33" s="10" t="s">
+      <c r="P33" s="10" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="34" spans="1:15" ht="30" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:16" ht="30" x14ac:dyDescent="0.25">
       <c r="A34" s="13" t="s">
         <v>36</v>
       </c>
@@ -5545,13 +5779,16 @@
         <v>39</v>
       </c>
       <c r="N34" s="5" t="s">
+        <v>105</v>
+      </c>
+      <c r="O34" s="5" t="s">
         <v>78</v>
       </c>
-      <c r="O34" s="9">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="35" spans="1:15" ht="30" x14ac:dyDescent="0.25">
+      <c r="P34" s="9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35" spans="1:16" ht="30" x14ac:dyDescent="0.25">
       <c r="A35" s="13" t="s">
         <v>36</v>
       </c>
@@ -5582,13 +5819,16 @@
         <v>39</v>
       </c>
       <c r="N35" s="5" t="s">
+        <v>105</v>
+      </c>
+      <c r="O35" s="5" t="s">
         <v>78</v>
       </c>
-      <c r="O35" s="9">
+      <c r="P35" s="9">
         <v>2</v>
       </c>
     </row>
-    <row r="36" spans="1:15" ht="30" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:16" ht="30" x14ac:dyDescent="0.25">
       <c r="A36" s="13" t="s">
         <v>36</v>
       </c>
@@ -5619,13 +5859,16 @@
         <v>39</v>
       </c>
       <c r="N36" s="5" t="s">
+        <v>105</v>
+      </c>
+      <c r="O36" s="5" t="s">
         <v>78</v>
       </c>
-      <c r="O36" s="9">
+      <c r="P36" s="9">
         <v>3</v>
       </c>
     </row>
-    <row r="37" spans="1:15" ht="30" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:16" ht="30" x14ac:dyDescent="0.25">
       <c r="A37" s="13" t="s">
         <v>36</v>
       </c>
@@ -5656,13 +5899,16 @@
         <v>39</v>
       </c>
       <c r="N37" s="5" t="s">
+        <v>105</v>
+      </c>
+      <c r="O37" s="5" t="s">
         <v>78</v>
       </c>
-      <c r="O37" s="9">
+      <c r="P37" s="9">
         <v>4</v>
       </c>
     </row>
-    <row r="38" spans="1:15" ht="30" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:16" ht="30" x14ac:dyDescent="0.25">
       <c r="A38" s="13" t="s">
         <v>36</v>
       </c>
@@ -5693,9 +5939,12 @@
         <v>39</v>
       </c>
       <c r="N38" s="5" t="s">
+        <v>105</v>
+      </c>
+      <c r="O38" s="5" t="s">
         <v>78</v>
       </c>
-      <c r="O38" s="9">
+      <c r="P38" s="9">
         <v>5</v>
       </c>
     </row>
@@ -6381,10 +6630,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O2"/>
+  <dimension ref="A1:P2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+    <sheetView topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="L13" sqref="L13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6400,12 +6649,12 @@
     <col min="10" max="10" width="22.5703125" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="16.140625" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="18" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="18" customWidth="1"/>
-    <col min="14" max="14" width="22.28515625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="20.5703125" bestFit="1" customWidth="1"/>
+    <col min="13" max="14" width="18" customWidth="1"/>
+    <col min="15" max="15" width="22.28515625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="20.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -6446,13 +6695,16 @@
         <v>15</v>
       </c>
       <c r="N1" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="O1" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="O1" s="3" t="s">
+      <c r="P1" s="3" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:15" ht="30" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:16" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="12" t="s">
         <v>88</v>
       </c>
@@ -6484,8 +6736,11 @@
       <c r="M2" s="9" t="s">
         <v>38</v>
       </c>
-      <c r="N2" s="5"/>
-      <c r="O2" s="17"/>
+      <c r="N2" s="5" t="s">
+        <v>105</v>
+      </c>
+      <c r="O2" s="5"/>
+      <c r="P2" s="17"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -6497,10 +6752,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O5"/>
+  <dimension ref="A1:P5"/>
   <sheetViews>
-    <sheetView topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="G20" sqref="G20"/>
+    <sheetView topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="L13" sqref="L13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6516,12 +6771,12 @@
     <col min="10" max="10" width="22.5703125" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="16.140625" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="18" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="18" customWidth="1"/>
-    <col min="14" max="14" width="22.28515625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="20.5703125" bestFit="1" customWidth="1"/>
+    <col min="13" max="14" width="18" customWidth="1"/>
+    <col min="15" max="15" width="22.28515625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="20.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -6562,18 +6817,21 @@
         <v>15</v>
       </c>
       <c r="N1" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="O1" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="O1" s="3" t="s">
+      <c r="P1" s="3" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2" s="12" t="s">
         <v>16</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>94</v>
+        <v>103</v>
       </c>
       <c r="C2" s="4">
         <v>35</v>
@@ -6600,10 +6858,13 @@
       <c r="M2" s="9" t="s">
         <v>38</v>
       </c>
-      <c r="N2" s="5"/>
-      <c r="O2" s="17"/>
-    </row>
-    <row r="3" spans="1:15" ht="30" x14ac:dyDescent="0.25">
+      <c r="N2" s="5" t="s">
+        <v>105</v>
+      </c>
+      <c r="O2" s="5"/>
+      <c r="P2" s="17"/>
+    </row>
+    <row r="3" spans="1:16" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="12" t="s">
         <v>19</v>
       </c>
@@ -6641,10 +6902,13 @@
       <c r="M3" s="9" t="s">
         <v>38</v>
       </c>
-      <c r="N3" s="5"/>
-      <c r="O3" s="17"/>
-    </row>
-    <row r="4" spans="1:15" ht="30" x14ac:dyDescent="0.25">
+      <c r="N3" s="5" t="s">
+        <v>105</v>
+      </c>
+      <c r="O3" s="5"/>
+      <c r="P3" s="17"/>
+    </row>
+    <row r="4" spans="1:16" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" s="12" t="s">
         <v>22</v>
       </c>
@@ -6680,10 +6944,13 @@
       <c r="M4" s="9" t="s">
         <v>39</v>
       </c>
-      <c r="N4" s="5"/>
-      <c r="O4" s="17"/>
-    </row>
-    <row r="5" spans="1:15" ht="30" x14ac:dyDescent="0.25">
+      <c r="N4" s="5" t="s">
+        <v>105</v>
+      </c>
+      <c r="O4" s="5"/>
+      <c r="P4" s="17"/>
+    </row>
+    <row r="5" spans="1:16" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" s="12" t="s">
         <v>91</v>
       </c>
@@ -6717,8 +6984,11 @@
       <c r="M5" s="9" t="s">
         <v>38</v>
       </c>
-      <c r="N5" s="5"/>
-      <c r="O5" s="17"/>
+      <c r="N5" s="5" t="s">
+        <v>105</v>
+      </c>
+      <c r="O5" s="5"/>
+      <c r="P5" s="17"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -6730,10 +7000,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O3"/>
+  <dimension ref="A1:P3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="N3" sqref="N3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6749,12 +7019,12 @@
     <col min="10" max="10" width="22.5703125" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="16.140625" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="18" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="18" customWidth="1"/>
-    <col min="14" max="14" width="22.28515625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="20.5703125" bestFit="1" customWidth="1"/>
+    <col min="13" max="14" width="18" customWidth="1"/>
+    <col min="15" max="15" width="22.28515625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="20.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -6795,13 +7065,16 @@
         <v>15</v>
       </c>
       <c r="N1" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="O1" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="O1" s="3" t="s">
+      <c r="P1" s="3" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2" s="12" t="s">
         <v>20</v>
       </c>
@@ -6835,10 +7108,13 @@
       <c r="M2" s="9" t="s">
         <v>39</v>
       </c>
-      <c r="N2" s="5"/>
-      <c r="O2" s="17"/>
-    </row>
-    <row r="3" spans="1:15" ht="30" x14ac:dyDescent="0.25">
+      <c r="N2" s="5" t="s">
+        <v>105</v>
+      </c>
+      <c r="O2" s="5"/>
+      <c r="P2" s="17"/>
+    </row>
+    <row r="3" spans="1:16" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="12" t="s">
         <v>87</v>
       </c>
@@ -6870,8 +7146,11 @@
       <c r="M3" s="9" t="s">
         <v>39</v>
       </c>
-      <c r="N3" s="5"/>
-      <c r="O3" s="17"/>
+      <c r="N3" s="5" t="s">
+        <v>105</v>
+      </c>
+      <c r="O3" s="5"/>
+      <c r="P3" s="17"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -6883,10 +7162,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O4"/>
+  <dimension ref="A1:P4"/>
   <sheetViews>
     <sheetView topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="N4" sqref="N4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6902,12 +7181,12 @@
     <col min="10" max="10" width="22.5703125" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="16.140625" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="18" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="18" customWidth="1"/>
-    <col min="14" max="14" width="22.28515625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="20.5703125" bestFit="1" customWidth="1"/>
+    <col min="13" max="14" width="18" customWidth="1"/>
+    <col min="15" max="15" width="22.28515625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="20.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -6948,13 +7227,16 @@
         <v>15</v>
       </c>
       <c r="N1" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="O1" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="O1" s="3" t="s">
+      <c r="P1" s="3" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2" s="12" t="s">
         <v>18</v>
       </c>
@@ -6988,10 +7270,13 @@
       <c r="M2" s="9" t="s">
         <v>39</v>
       </c>
-      <c r="N2" s="5"/>
-      <c r="O2" s="17"/>
-    </row>
-    <row r="3" spans="1:15" ht="30" x14ac:dyDescent="0.25">
+      <c r="N2" s="5" t="s">
+        <v>105</v>
+      </c>
+      <c r="O2" s="5"/>
+      <c r="P2" s="17"/>
+    </row>
+    <row r="3" spans="1:16" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="12" t="s">
         <v>89</v>
       </c>
@@ -7023,10 +7308,13 @@
       <c r="M3" s="9" t="s">
         <v>38</v>
       </c>
-      <c r="N3" s="5"/>
-      <c r="O3" s="17"/>
-    </row>
-    <row r="4" spans="1:15" ht="30" x14ac:dyDescent="0.25">
+      <c r="N3" s="5" t="s">
+        <v>105</v>
+      </c>
+      <c r="O3" s="5"/>
+      <c r="P3" s="17"/>
+    </row>
+    <row r="4" spans="1:16" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" s="12" t="s">
         <v>90</v>
       </c>
@@ -7060,8 +7348,11 @@
       <c r="M4" s="9" t="s">
         <v>38</v>
       </c>
-      <c r="N4" s="5"/>
-      <c r="O4" s="17"/>
+      <c r="N4" s="5" t="s">
+        <v>105</v>
+      </c>
+      <c r="O4" s="5"/>
+      <c r="P4" s="17"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -7073,10 +7364,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O3"/>
+  <dimension ref="A1:P3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="L12" sqref="L12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7092,12 +7383,12 @@
     <col min="10" max="10" width="22.5703125" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="16.140625" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="18" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="18" customWidth="1"/>
-    <col min="14" max="14" width="22.28515625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="20.5703125" bestFit="1" customWidth="1"/>
+    <col min="13" max="14" width="18" customWidth="1"/>
+    <col min="15" max="15" width="22.28515625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="20.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -7138,13 +7429,16 @@
         <v>15</v>
       </c>
       <c r="N1" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="O1" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="O1" s="3" t="s">
+      <c r="P1" s="3" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2" s="12" t="s">
         <v>17</v>
       </c>
@@ -7181,9 +7475,10 @@
         <v>39</v>
       </c>
       <c r="N2" s="5"/>
-      <c r="O2" s="17"/>
-    </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="O2" s="5"/>
+      <c r="P2" s="17"/>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A3" s="12" t="s">
         <v>41</v>
       </c>
@@ -7222,7 +7517,8 @@
         <v>39</v>
       </c>
       <c r="N3" s="5"/>
-      <c r="O3" s="17"/>
+      <c r="O3" s="5"/>
+      <c r="P3" s="17"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -7234,10 +7530,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O4"/>
+  <dimension ref="A1:P4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B38" sqref="B38"/>
+    <sheetView topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="L18" sqref="L18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7253,12 +7549,12 @@
     <col min="10" max="10" width="22.5703125" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="16.140625" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="18" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="18" customWidth="1"/>
-    <col min="14" max="14" width="22.28515625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="20.5703125" bestFit="1" customWidth="1"/>
+    <col min="13" max="14" width="18" customWidth="1"/>
+    <col min="15" max="15" width="22.28515625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="20.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -7299,13 +7595,16 @@
         <v>15</v>
       </c>
       <c r="N1" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="O1" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="O1" s="3" t="s">
+      <c r="P1" s="3" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:15" ht="30" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:16" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="12" t="s">
         <v>23</v>
       </c>
@@ -7338,9 +7637,10 @@
         <v>39</v>
       </c>
       <c r="N2" s="5"/>
-      <c r="O2" s="17"/>
-    </row>
-    <row r="3" spans="1:15" ht="30" x14ac:dyDescent="0.25">
+      <c r="O2" s="5"/>
+      <c r="P2" s="17"/>
+    </row>
+    <row r="3" spans="1:16" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="12" t="s">
         <v>50</v>
       </c>
@@ -7375,9 +7675,10 @@
         <v>39</v>
       </c>
       <c r="N3" s="5"/>
-      <c r="O3" s="17"/>
-    </row>
-    <row r="4" spans="1:15" ht="30" x14ac:dyDescent="0.25">
+      <c r="O3" s="5"/>
+      <c r="P3" s="17"/>
+    </row>
+    <row r="4" spans="1:16" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" s="12" t="s">
         <v>92</v>
       </c>
@@ -7412,7 +7713,8 @@
         <v>38</v>
       </c>
       <c r="N4" s="5"/>
-      <c r="O4" s="17"/>
+      <c r="O4" s="5"/>
+      <c r="P4" s="17"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -7424,10 +7726,10 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O7"/>
+  <dimension ref="A1:P7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="L14" sqref="L14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7443,12 +7745,12 @@
     <col min="10" max="10" width="22.5703125" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="16.140625" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="18" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="18" customWidth="1"/>
-    <col min="14" max="14" width="22.28515625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="20.5703125" bestFit="1" customWidth="1"/>
+    <col min="13" max="14" width="18" customWidth="1"/>
+    <col min="15" max="15" width="22.28515625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="20.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -7489,13 +7791,16 @@
         <v>15</v>
       </c>
       <c r="N1" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="O1" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="O1" s="3" t="s">
+      <c r="P1" s="3" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2" s="12" t="s">
         <v>21</v>
       </c>
@@ -7530,9 +7835,10 @@
         <v>39</v>
       </c>
       <c r="N2" s="5"/>
-      <c r="O2" s="17"/>
-    </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="O2" s="5"/>
+      <c r="P2" s="17"/>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A3" s="12" t="s">
         <v>42</v>
       </c>
@@ -7569,9 +7875,10 @@
         <v>39</v>
       </c>
       <c r="N3" s="5"/>
-      <c r="O3" s="17"/>
-    </row>
-    <row r="4" spans="1:15" ht="30" x14ac:dyDescent="0.25">
+      <c r="O3" s="5"/>
+      <c r="P3" s="17"/>
+    </row>
+    <row r="4" spans="1:16" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" s="12" t="s">
         <v>43</v>
       </c>
@@ -7610,9 +7917,10 @@
         <v>39</v>
       </c>
       <c r="N4" s="5"/>
-      <c r="O4" s="17"/>
-    </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="O4" s="5"/>
+      <c r="P4" s="17"/>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A5" s="12" t="s">
         <v>44</v>
       </c>
@@ -7649,9 +7957,10 @@
         <v>39</v>
       </c>
       <c r="N5" s="5"/>
-      <c r="O5" s="17"/>
-    </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="O5" s="5"/>
+      <c r="P5" s="17"/>
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A6" s="12" t="s">
         <v>24</v>
       </c>
@@ -7686,9 +7995,10 @@
         <v>39</v>
       </c>
       <c r="N6" s="5"/>
-      <c r="O6" s="17"/>
-    </row>
-    <row r="7" spans="1:15" ht="30" x14ac:dyDescent="0.25">
+      <c r="O6" s="5"/>
+      <c r="P6" s="17"/>
+    </row>
+    <row r="7" spans="1:16" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" s="12" t="s">
         <v>51</v>
       </c>
@@ -7725,7 +8035,8 @@
         <v>39</v>
       </c>
       <c r="N7" s="5"/>
-      <c r="O7" s="17"/>
+      <c r="O7" s="5"/>
+      <c r="P7" s="17"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -7737,10 +8048,10 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O17"/>
+  <dimension ref="A1:P17"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="N8" sqref="N8"/>
+      <selection activeCell="N1" sqref="N1:N1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7756,12 +8067,12 @@
     <col min="10" max="10" width="22.5703125" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="16.140625" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="18" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="18" customWidth="1"/>
-    <col min="14" max="14" width="22.28515625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="25.7109375" bestFit="1" customWidth="1"/>
+    <col min="13" max="14" width="18" customWidth="1"/>
+    <col min="15" max="15" width="22.28515625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="25.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -7802,13 +8113,16 @@
         <v>15</v>
       </c>
       <c r="N1" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="O1" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="O1" s="3" t="s">
+      <c r="P1" s="3" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:15" ht="30" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:16" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="13" t="s">
         <v>25</v>
       </c>
@@ -7838,14 +8152,15 @@
       <c r="M2" s="9" t="s">
         <v>39</v>
       </c>
-      <c r="N2" s="5" t="s">
+      <c r="N2" s="5"/>
+      <c r="O2" s="5" t="s">
         <v>100</v>
       </c>
-      <c r="O2" s="16" t="s">
+      <c r="P2" s="16" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="3" spans="1:15" ht="30" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:16" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="13" t="s">
         <v>26</v>
       </c>
@@ -7875,14 +8190,15 @@
       <c r="M3" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="N3" s="5" t="s">
+      <c r="N3" s="5"/>
+      <c r="O3" s="5" t="s">
         <v>74</v>
       </c>
-      <c r="O3" s="6" t="s">
+      <c r="P3" s="6" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="4" spans="1:15" ht="30" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:16" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" s="13" t="s">
         <v>27</v>
       </c>
@@ -7912,14 +8228,15 @@
       <c r="M4" s="9" t="s">
         <v>39</v>
       </c>
-      <c r="N4" s="5" t="s">
+      <c r="N4" s="5"/>
+      <c r="O4" s="5" t="s">
         <v>72</v>
       </c>
-      <c r="O4" s="17" t="s">
+      <c r="P4" s="17" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="5" spans="1:15" ht="30" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:16" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" s="14" t="s">
         <v>28</v>
       </c>
@@ -7949,14 +8266,15 @@
       <c r="M5" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="N5" s="5" t="s">
+      <c r="N5" s="5"/>
+      <c r="O5" s="5" t="s">
         <v>102</v>
       </c>
-      <c r="O5" s="10" t="s">
+      <c r="P5" s="10" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="6" spans="1:15" ht="30" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:16" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" s="14" t="s">
         <v>29</v>
       </c>
@@ -7986,14 +8304,15 @@
       <c r="M6" s="9" t="s">
         <v>39</v>
       </c>
-      <c r="N6" s="5" t="s">
+      <c r="N6" s="5"/>
+      <c r="O6" s="5" t="s">
         <v>76</v>
       </c>
-      <c r="O6" s="11" t="s">
+      <c r="P6" s="11" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="7" spans="1:15" ht="30" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:16" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" s="13" t="s">
         <v>30</v>
       </c>
@@ -8023,14 +8342,15 @@
       <c r="M7" s="9" t="s">
         <v>39</v>
       </c>
-      <c r="N7" s="5" t="s">
+      <c r="N7" s="5"/>
+      <c r="O7" s="5" t="s">
         <v>77</v>
       </c>
-      <c r="O7" s="10" t="s">
+      <c r="P7" s="10" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="8" spans="1:15" ht="30" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:16" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" s="13" t="s">
         <v>31</v>
       </c>
@@ -8060,14 +8380,15 @@
       <c r="M8" s="9" t="s">
         <v>39</v>
       </c>
-      <c r="N8" s="5" t="s">
+      <c r="N8" s="5"/>
+      <c r="O8" s="5" t="s">
         <v>77</v>
       </c>
-      <c r="O8" s="10" t="s">
+      <c r="P8" s="10" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="9" spans="1:15" ht="30" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:16" ht="30" x14ac:dyDescent="0.25">
       <c r="A9" s="13" t="s">
         <v>32</v>
       </c>
@@ -8097,14 +8418,15 @@
       <c r="M9" s="9" t="s">
         <v>39</v>
       </c>
-      <c r="N9" s="5" t="s">
+      <c r="N9" s="5"/>
+      <c r="O9" s="5" t="s">
         <v>77</v>
       </c>
-      <c r="O9" s="10" t="s">
+      <c r="P9" s="10" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="10" spans="1:15" ht="30" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:16" ht="30" x14ac:dyDescent="0.25">
       <c r="A10" s="13" t="s">
         <v>33</v>
       </c>
@@ -8134,14 +8456,15 @@
       <c r="M10" s="9" t="s">
         <v>39</v>
       </c>
-      <c r="N10" s="5" t="s">
+      <c r="N10" s="5"/>
+      <c r="O10" s="5" t="s">
         <v>77</v>
       </c>
-      <c r="O10" s="10" t="s">
+      <c r="P10" s="10" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="11" spans="1:15" ht="30" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:16" ht="30" x14ac:dyDescent="0.25">
       <c r="A11" s="13" t="s">
         <v>34</v>
       </c>
@@ -8171,14 +8494,15 @@
       <c r="M11" s="9" t="s">
         <v>39</v>
       </c>
-      <c r="N11" s="5" t="s">
+      <c r="N11" s="5"/>
+      <c r="O11" s="5" t="s">
         <v>77</v>
       </c>
-      <c r="O11" s="10" t="s">
+      <c r="P11" s="10" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="12" spans="1:15" ht="30" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:16" ht="30" x14ac:dyDescent="0.25">
       <c r="A12" s="13" t="s">
         <v>35</v>
       </c>
@@ -8208,14 +8532,15 @@
       <c r="M12" s="9" t="s">
         <v>39</v>
       </c>
-      <c r="N12" s="5" t="s">
+      <c r="N12" s="5"/>
+      <c r="O12" s="5" t="s">
         <v>77</v>
       </c>
-      <c r="O12" s="10" t="s">
+      <c r="P12" s="10" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="13" spans="1:15" ht="30" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:16" ht="30" x14ac:dyDescent="0.25">
       <c r="A13" s="13" t="s">
         <v>36</v>
       </c>
@@ -8245,14 +8570,15 @@
       <c r="M13" s="9" t="s">
         <v>39</v>
       </c>
-      <c r="N13" s="5" t="s">
+      <c r="N13" s="5"/>
+      <c r="O13" s="5" t="s">
         <v>78</v>
       </c>
-      <c r="O13" s="9">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="14" spans="1:15" ht="30" x14ac:dyDescent="0.25">
+      <c r="P13" s="9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:16" ht="30" x14ac:dyDescent="0.25">
       <c r="A14" s="13" t="s">
         <v>36</v>
       </c>
@@ -8282,14 +8608,15 @@
       <c r="M14" s="9" t="s">
         <v>39</v>
       </c>
-      <c r="N14" s="5" t="s">
+      <c r="N14" s="5"/>
+      <c r="O14" s="5" t="s">
         <v>78</v>
       </c>
-      <c r="O14" s="9">
+      <c r="P14" s="9">
         <v>2</v>
       </c>
     </row>
-    <row r="15" spans="1:15" ht="30" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:16" ht="30" x14ac:dyDescent="0.25">
       <c r="A15" s="13" t="s">
         <v>36</v>
       </c>
@@ -8319,14 +8646,15 @@
       <c r="M15" s="9" t="s">
         <v>39</v>
       </c>
-      <c r="N15" s="5" t="s">
+      <c r="N15" s="5"/>
+      <c r="O15" s="5" t="s">
         <v>78</v>
       </c>
-      <c r="O15" s="9">
+      <c r="P15" s="9">
         <v>3</v>
       </c>
     </row>
-    <row r="16" spans="1:15" ht="30" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:16" ht="30" x14ac:dyDescent="0.25">
       <c r="A16" s="13" t="s">
         <v>36</v>
       </c>
@@ -8356,14 +8684,15 @@
       <c r="M16" s="9" t="s">
         <v>39</v>
       </c>
-      <c r="N16" s="5" t="s">
+      <c r="N16" s="5"/>
+      <c r="O16" s="5" t="s">
         <v>78</v>
       </c>
-      <c r="O16" s="9">
+      <c r="P16" s="9">
         <v>4</v>
       </c>
     </row>
-    <row r="17" spans="1:15" ht="30" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:16" ht="30" x14ac:dyDescent="0.25">
       <c r="A17" s="13" t="s">
         <v>36</v>
       </c>
@@ -8393,10 +8722,11 @@
       <c r="M17" s="9" t="s">
         <v>39</v>
       </c>
-      <c r="N17" s="5" t="s">
+      <c r="N17" s="5"/>
+      <c r="O17" s="5" t="s">
         <v>78</v>
       </c>
-      <c r="O17" s="9">
+      <c r="P17" s="9">
         <v>5</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Added Pay Now Implementation and Confirmation Page validation for Activity
</commit_message>
<xml_diff>
--- a/Rovia.UI.Automation.Tests/DataSheet/Hotel/HotelScenarios.xlsx
+++ b/Rovia.UI.Automation.Tests/DataSheet/Hotel/HotelScenarios.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="801" uniqueCount="104">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="801" uniqueCount="106">
   <si>
     <t>Description</t>
   </si>
@@ -335,6 +335,12 @@
   </si>
   <si>
     <t>CreditCard</t>
+  </si>
+  <si>
+    <t>NameDsc</t>
+  </si>
+  <si>
+    <t>NameAsc</t>
   </si>
 </sst>
 </file>
@@ -818,30 +824,30 @@
       </border>
     </dxf>
     <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
       <border>
         <bottom style="thin">
           <color indexed="64"/>
         </bottom>
       </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <border diagonalUp="0" diagonalDown="0">
@@ -3852,28 +3858,28 @@
 </file>
 
 <file path=xl/tables/table10.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="11" name="Table210111012" displayName="Table210111012" ref="A1:P17" totalsRowShown="0" headerRowDxfId="41" dataDxfId="39" headerRowBorderDxfId="40" tableBorderDxfId="38" totalsRowBorderDxfId="37">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="11" name="Table210111012" displayName="Table210111012" ref="A1:P17" totalsRowShown="0" headerRowDxfId="20" dataDxfId="18" headerRowBorderDxfId="19" tableBorderDxfId="17" totalsRowBorderDxfId="16">
   <autoFilter ref="A1:P17"/>
   <sortState ref="A2:O38">
     <sortCondition ref="L1:L38"/>
   </sortState>
   <tableColumns count="16">
-    <tableColumn id="1" name="Description" dataDxfId="36"/>
-    <tableColumn id="16" name="ExecutionPipeLine" dataDxfId="35"/>
-    <tableColumn id="17" name="CheckInDate" dataDxfId="34"/>
-    <tableColumn id="18" name="CheckOutDate" dataDxfId="33"/>
-    <tableColumn id="3" name="ShortLocation" dataDxfId="32"/>
-    <tableColumn id="4" name="Location" dataDxfId="31"/>
-    <tableColumn id="5" name="Adults" dataDxfId="30"/>
-    <tableColumn id="6" name="ChildrenAges" dataDxfId="29"/>
-    <tableColumn id="8" name="AdditionalPreferences" dataDxfId="28"/>
-    <tableColumn id="9" name="HotelName" dataDxfId="27"/>
-    <tableColumn id="10" name="StarRating" dataDxfId="26"/>
-    <tableColumn id="11" name="Supplier" dataDxfId="25"/>
-    <tableColumn id="7" name="UserType" dataDxfId="24"/>
-    <tableColumn id="2" name="PaymentMode" dataDxfId="23"/>
-    <tableColumn id="14" name="PostSearchFilters" dataDxfId="22"/>
-    <tableColumn id="15" name="PostSearchFilterValues" dataDxfId="21"/>
+    <tableColumn id="1" name="Description" dataDxfId="15"/>
+    <tableColumn id="16" name="ExecutionPipeLine" dataDxfId="14"/>
+    <tableColumn id="17" name="CheckInDate" dataDxfId="13"/>
+    <tableColumn id="18" name="CheckOutDate" dataDxfId="12"/>
+    <tableColumn id="3" name="ShortLocation" dataDxfId="11"/>
+    <tableColumn id="4" name="Location" dataDxfId="10"/>
+    <tableColumn id="5" name="Adults" dataDxfId="9"/>
+    <tableColumn id="6" name="ChildrenAges" dataDxfId="8"/>
+    <tableColumn id="8" name="AdditionalPreferences" dataDxfId="7"/>
+    <tableColumn id="9" name="HotelName" dataDxfId="6"/>
+    <tableColumn id="10" name="StarRating" dataDxfId="5"/>
+    <tableColumn id="11" name="Supplier" dataDxfId="4"/>
+    <tableColumn id="7" name="UserType" dataDxfId="3"/>
+    <tableColumn id="2" name="PaymentMode" dataDxfId="2"/>
+    <tableColumn id="14" name="PostSearchFilters" dataDxfId="1"/>
+    <tableColumn id="15" name="PostSearchFilterValues" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -4076,28 +4082,28 @@
 </file>
 
 <file path=xl/tables/table9.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="10" name="Table21011101211" displayName="Table21011101211" ref="A1:P17" totalsRowShown="0" headerRowDxfId="20" dataDxfId="19" headerRowBorderDxfId="17" tableBorderDxfId="18" totalsRowBorderDxfId="16">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="10" name="Table21011101211" displayName="Table21011101211" ref="A1:P17" totalsRowShown="0" headerRowDxfId="41" dataDxfId="39" headerRowBorderDxfId="40" tableBorderDxfId="38" totalsRowBorderDxfId="37">
   <autoFilter ref="A1:P17"/>
   <sortState ref="A2:O38">
     <sortCondition ref="L1:L38"/>
   </sortState>
   <tableColumns count="16">
-    <tableColumn id="1" name="Description" dataDxfId="15"/>
-    <tableColumn id="16" name="ExecutionPipeLine" dataDxfId="14"/>
-    <tableColumn id="17" name="CheckInDate" dataDxfId="13"/>
-    <tableColumn id="18" name="CheckOutDate" dataDxfId="12"/>
-    <tableColumn id="3" name="ShortLocation" dataDxfId="11"/>
-    <tableColumn id="4" name="Location" dataDxfId="10"/>
-    <tableColumn id="5" name="Adults" dataDxfId="9"/>
-    <tableColumn id="6" name="ChildrenAges" dataDxfId="8"/>
-    <tableColumn id="8" name="AdditionalPreferences" dataDxfId="7"/>
-    <tableColumn id="9" name="HotelName" dataDxfId="6"/>
-    <tableColumn id="10" name="StarRating" dataDxfId="5"/>
-    <tableColumn id="11" name="Supplier" dataDxfId="4"/>
-    <tableColumn id="7" name="UserType" dataDxfId="3"/>
-    <tableColumn id="2" name="PaymentMode" dataDxfId="2"/>
-    <tableColumn id="14" name="PostSearchFilters" dataDxfId="1"/>
-    <tableColumn id="15" name="PostSearchFilterValues" dataDxfId="0"/>
+    <tableColumn id="1" name="Description" dataDxfId="36"/>
+    <tableColumn id="16" name="ExecutionPipeLine" dataDxfId="35"/>
+    <tableColumn id="17" name="CheckInDate" dataDxfId="34"/>
+    <tableColumn id="18" name="CheckOutDate" dataDxfId="33"/>
+    <tableColumn id="3" name="ShortLocation" dataDxfId="32"/>
+    <tableColumn id="4" name="Location" dataDxfId="31"/>
+    <tableColumn id="5" name="Adults" dataDxfId="30"/>
+    <tableColumn id="6" name="ChildrenAges" dataDxfId="29"/>
+    <tableColumn id="8" name="AdditionalPreferences" dataDxfId="28"/>
+    <tableColumn id="9" name="HotelName" dataDxfId="27"/>
+    <tableColumn id="10" name="StarRating" dataDxfId="26"/>
+    <tableColumn id="11" name="Supplier" dataDxfId="25"/>
+    <tableColumn id="7" name="UserType" dataDxfId="24"/>
+    <tableColumn id="2" name="PaymentMode" dataDxfId="23"/>
+    <tableColumn id="14" name="PostSearchFilters" dataDxfId="22"/>
+    <tableColumn id="15" name="PostSearchFilterValues" dataDxfId="21"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -8079,8 +8085,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D21" sqref="D21"/>
+    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
+      <selection activeCell="P10" sqref="P10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8452,7 +8458,7 @@
         <v>77</v>
       </c>
       <c r="P9" s="10" t="s">
-        <v>81</v>
+        <v>105</v>
       </c>
     </row>
     <row r="10" spans="1:16" ht="30" x14ac:dyDescent="0.25">
@@ -8490,7 +8496,7 @@
         <v>77</v>
       </c>
       <c r="P10" s="10" t="s">
-        <v>82</v>
+        <v>104</v>
       </c>
     </row>
     <row r="11" spans="1:16" ht="30" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Location name updated in hotel
</commit_message>
<xml_diff>
--- a/Rovia.UI.Automation.Tests/DataSheet/Hotel/HotelScenarios.xlsx
+++ b/Rovia.UI.Automation.Tests/DataSheet/Hotel/HotelScenarios.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="225" windowWidth="14805" windowHeight="7890" tabRatio="722" firstSheet="3" activeTab="8"/>
+    <workbookView xWindow="240" yWindow="225" windowWidth="14805" windowHeight="7890" tabRatio="722" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="GeneralScenarios" sheetId="1" r:id="rId1"/>
@@ -316,9 +316,6 @@
     <t>Country Inn &amp; Suites By Carlson Roseville MN.. US</t>
   </si>
   <si>
-    <t>Country Inn &amp; Suites By Carlson Roseville.. MN.. US</t>
-  </si>
-  <si>
     <t>El Cortez Hotel and Casino</t>
   </si>
   <si>
@@ -341,6 +338,9 @@
   </si>
   <si>
     <t>NameAsc</t>
+  </si>
+  <si>
+    <t>Country Inn &amp; Suites By Carlson Roseville MN.. MN.. US</t>
   </si>
 </sst>
 </file>
@@ -4463,7 +4463,7 @@
         <v>15</v>
       </c>
       <c r="N1" s="3" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="O1" s="3" t="s">
         <v>13</v>
@@ -4497,7 +4497,7 @@
       <c r="H2" s="4"/>
       <c r="I2" s="10"/>
       <c r="J2" s="10" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="K2" s="4"/>
       <c r="L2" s="10"/>
@@ -4505,7 +4505,7 @@
         <v>38</v>
       </c>
       <c r="N2" s="5" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="O2" s="5"/>
       <c r="P2" s="17"/>
@@ -4545,7 +4545,7 @@
         <v>39</v>
       </c>
       <c r="N3" s="5" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="O3" s="5"/>
       <c r="P3" s="17"/>
@@ -4583,7 +4583,7 @@
         <v>39</v>
       </c>
       <c r="N4" s="5" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="O4" s="5"/>
       <c r="P4" s="17"/>
@@ -4621,7 +4621,7 @@
         <v>38</v>
       </c>
       <c r="N5" s="5" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="O5" s="5"/>
       <c r="P5" s="17"/>
@@ -4665,7 +4665,7 @@
         <v>38</v>
       </c>
       <c r="N6" s="5" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="O6" s="5"/>
       <c r="P6" s="17"/>
@@ -4707,7 +4707,7 @@
         <v>39</v>
       </c>
       <c r="N7" s="5" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="O7" s="5"/>
       <c r="P7" s="17"/>
@@ -4747,7 +4747,7 @@
         <v>38</v>
       </c>
       <c r="N8" s="5" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="O8" s="5"/>
       <c r="P8" s="17"/>
@@ -4787,7 +4787,7 @@
         <v>39</v>
       </c>
       <c r="N9" s="5" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="O9" s="5"/>
       <c r="P9" s="17"/>
@@ -4825,7 +4825,7 @@
         <v>38</v>
       </c>
       <c r="N10" s="5" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="O10" s="5"/>
       <c r="P10" s="17"/>
@@ -4865,7 +4865,7 @@
         <v>38</v>
       </c>
       <c r="N11" s="5" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="O11" s="5"/>
       <c r="P11" s="17"/>
@@ -4907,7 +4907,7 @@
         <v>39</v>
       </c>
       <c r="N12" s="5" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="O12" s="5"/>
       <c r="P12" s="17"/>
@@ -4951,7 +4951,7 @@
         <v>39</v>
       </c>
       <c r="N13" s="5" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="O13" s="5"/>
       <c r="P13" s="17"/>
@@ -4989,7 +4989,7 @@
         <v>39</v>
       </c>
       <c r="N14" s="5" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="O14" s="5"/>
       <c r="P14" s="17"/>
@@ -5029,7 +5029,7 @@
         <v>39</v>
       </c>
       <c r="N15" s="5" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="O15" s="5"/>
       <c r="P15" s="17"/>
@@ -5069,7 +5069,7 @@
         <v>38</v>
       </c>
       <c r="N16" s="5" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="O16" s="5"/>
       <c r="P16" s="17"/>
@@ -5109,7 +5109,7 @@
         <v>39</v>
       </c>
       <c r="N17" s="5" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="O17" s="5"/>
       <c r="P17" s="17"/>
@@ -5151,7 +5151,7 @@
         <v>39</v>
       </c>
       <c r="N18" s="5" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="O18" s="5"/>
       <c r="P18" s="17"/>
@@ -5195,7 +5195,7 @@
         <v>39</v>
       </c>
       <c r="N19" s="5" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="O19" s="5"/>
       <c r="P19" s="17"/>
@@ -5237,7 +5237,7 @@
         <v>39</v>
       </c>
       <c r="N20" s="5" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="O20" s="5"/>
       <c r="P20" s="17"/>
@@ -5277,7 +5277,7 @@
         <v>39</v>
       </c>
       <c r="N21" s="5" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="O21" s="5"/>
       <c r="P21" s="17"/>
@@ -5319,7 +5319,7 @@
         <v>39</v>
       </c>
       <c r="N22" s="5" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="O22" s="5"/>
       <c r="P22" s="17"/>
@@ -5357,7 +5357,7 @@
         <v>39</v>
       </c>
       <c r="N23" s="5" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="O23" s="5"/>
       <c r="P23" s="17"/>
@@ -5393,7 +5393,7 @@
         <v>38</v>
       </c>
       <c r="N24" s="5" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="O24" s="5" t="s">
         <v>74</v>
@@ -5435,7 +5435,7 @@
         <v>39</v>
       </c>
       <c r="N25" s="5" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="O25" s="5" t="s">
         <v>72</v>
@@ -5477,7 +5477,7 @@
         <v>38</v>
       </c>
       <c r="N26" s="5" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="O26" s="5"/>
       <c r="P26" s="17"/>
@@ -5513,7 +5513,7 @@
         <v>39</v>
       </c>
       <c r="N27" s="5" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="O27" s="5" t="s">
         <v>76</v>
@@ -5553,7 +5553,7 @@
         <v>39</v>
       </c>
       <c r="N28" s="5" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="O28" s="5" t="s">
         <v>77</v>
@@ -5593,7 +5593,7 @@
         <v>39</v>
       </c>
       <c r="N29" s="5" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="O29" s="5" t="s">
         <v>77</v>
@@ -5633,7 +5633,7 @@
         <v>39</v>
       </c>
       <c r="N30" s="5" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="O30" s="5" t="s">
         <v>77</v>
@@ -5673,7 +5673,7 @@
         <v>39</v>
       </c>
       <c r="N31" s="5" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="O31" s="5" t="s">
         <v>77</v>
@@ -5713,7 +5713,7 @@
         <v>39</v>
       </c>
       <c r="N32" s="5" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="O32" s="5" t="s">
         <v>77</v>
@@ -5753,7 +5753,7 @@
         <v>39</v>
       </c>
       <c r="N33" s="5" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="O33" s="5" t="s">
         <v>77</v>
@@ -5793,7 +5793,7 @@
         <v>39</v>
       </c>
       <c r="N34" s="5" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="O34" s="5" t="s">
         <v>78</v>
@@ -5833,7 +5833,7 @@
         <v>39</v>
       </c>
       <c r="N35" s="5" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="O35" s="5" t="s">
         <v>78</v>
@@ -5873,7 +5873,7 @@
         <v>39</v>
       </c>
       <c r="N36" s="5" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="O36" s="5" t="s">
         <v>78</v>
@@ -5913,7 +5913,7 @@
         <v>39</v>
       </c>
       <c r="N37" s="5" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="O37" s="5" t="s">
         <v>78</v>
@@ -5953,7 +5953,7 @@
         <v>39</v>
       </c>
       <c r="N38" s="5" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="O38" s="5" t="s">
         <v>78</v>
@@ -6038,7 +6038,7 @@
         <v>15</v>
       </c>
       <c r="N1" s="3" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="O1" s="3" t="s">
         <v>13</v>
@@ -6079,7 +6079,7 @@
       </c>
       <c r="N2" s="5"/>
       <c r="O2" s="5" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="P2" s="16" t="s">
         <v>56</v>
@@ -6193,10 +6193,10 @@
       </c>
       <c r="N5" s="5"/>
       <c r="O5" s="5" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="P5" s="10" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="6" spans="1:16" ht="30" x14ac:dyDescent="0.25">
@@ -6667,8 +6667,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="L13" sqref="L13"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6730,7 +6730,7 @@
         <v>15</v>
       </c>
       <c r="N1" s="3" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="O1" s="3" t="s">
         <v>13</v>
@@ -6756,7 +6756,7 @@
         <v>96</v>
       </c>
       <c r="F2" s="16" t="s">
-        <v>97</v>
+        <v>105</v>
       </c>
       <c r="G2" s="4">
         <v>1</v>
@@ -6772,7 +6772,7 @@
         <v>38</v>
       </c>
       <c r="N2" s="5" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="O2" s="5"/>
       <c r="P2" s="17"/>
@@ -6852,7 +6852,7 @@
         <v>15</v>
       </c>
       <c r="N1" s="3" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="O1" s="3" t="s">
         <v>13</v>
@@ -6894,7 +6894,7 @@
         <v>38</v>
       </c>
       <c r="N2" s="5" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="O2" s="5"/>
       <c r="P2" s="17"/>
@@ -6938,7 +6938,7 @@
         <v>38</v>
       </c>
       <c r="N3" s="5" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="O3" s="5"/>
       <c r="P3" s="17"/>
@@ -6980,7 +6980,7 @@
         <v>39</v>
       </c>
       <c r="N4" s="5" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="O4" s="5"/>
       <c r="P4" s="17"/>
@@ -7020,7 +7020,7 @@
         <v>38</v>
       </c>
       <c r="N5" s="5" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="O5" s="5"/>
       <c r="P5" s="17"/>
@@ -7100,7 +7100,7 @@
         <v>15</v>
       </c>
       <c r="N1" s="3" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="O1" s="3" t="s">
         <v>13</v>
@@ -7144,7 +7144,7 @@
         <v>39</v>
       </c>
       <c r="N2" s="5" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="O2" s="5"/>
       <c r="P2" s="17"/>
@@ -7182,7 +7182,7 @@
         <v>39</v>
       </c>
       <c r="N3" s="5" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="O3" s="5"/>
       <c r="P3" s="17"/>
@@ -7262,7 +7262,7 @@
         <v>15</v>
       </c>
       <c r="N1" s="3" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="O1" s="3" t="s">
         <v>13</v>
@@ -7306,7 +7306,7 @@
         <v>39</v>
       </c>
       <c r="N2" s="5" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="O2" s="5"/>
       <c r="P2" s="17"/>
@@ -7344,7 +7344,7 @@
         <v>38</v>
       </c>
       <c r="N3" s="5" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="O3" s="5"/>
       <c r="P3" s="17"/>
@@ -7384,7 +7384,7 @@
         <v>38</v>
       </c>
       <c r="N4" s="5" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="O4" s="5"/>
       <c r="P4" s="17"/>
@@ -7464,7 +7464,7 @@
         <v>15</v>
       </c>
       <c r="N1" s="3" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="O1" s="3" t="s">
         <v>13</v>
@@ -7630,7 +7630,7 @@
         <v>15</v>
       </c>
       <c r="N1" s="3" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="O1" s="3" t="s">
         <v>13</v>
@@ -7826,7 +7826,7 @@
         <v>15</v>
       </c>
       <c r="N1" s="3" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="O1" s="3" t="s">
         <v>13</v>
@@ -8085,7 +8085,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P17"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
+    <sheetView topLeftCell="G1" workbookViewId="0">
       <selection activeCell="P10" sqref="P10"/>
     </sheetView>
   </sheetViews>
@@ -8148,7 +8148,7 @@
         <v>15</v>
       </c>
       <c r="N1" s="3" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="O1" s="3" t="s">
         <v>13</v>
@@ -8189,7 +8189,7 @@
       </c>
       <c r="N2" s="5"/>
       <c r="O2" s="5" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="P2" s="16" t="s">
         <v>56</v>
@@ -8303,10 +8303,10 @@
       </c>
       <c r="N5" s="5"/>
       <c r="O5" s="5" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="P5" s="10" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="6" spans="1:16" ht="30" x14ac:dyDescent="0.25">
@@ -8458,7 +8458,7 @@
         <v>77</v>
       </c>
       <c r="P9" s="10" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="10" spans="1:16" ht="30" x14ac:dyDescent="0.25">
@@ -8496,7 +8496,7 @@
         <v>77</v>
       </c>
       <c r="P10" s="10" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="11" spans="1:16" ht="30" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
updated hotel location in scenario
</commit_message>
<xml_diff>
--- a/Rovia.UI.Automation.Tests/DataSheet/Hotel/HotelScenarios.xlsx
+++ b/Rovia.UI.Automation.Tests/DataSheet/Hotel/HotelScenarios.xlsx
@@ -340,7 +340,7 @@
     <t>NameAsc</t>
   </si>
   <si>
-    <t>Country Inn &amp; Suites By Carlson Roseville MN.. MN.. US</t>
+    <t>Country Inn and Suites By Carlson Roseville MN.. MN.. US</t>
   </si>
 </sst>
 </file>
@@ -6668,7 +6668,7 @@
   <dimension ref="A1:P2"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>